<commit_message>
updated documents, tuned MIPGap
</commit_message>
<xml_diff>
--- a/doc/Time.xlsx
+++ b/doc/Time.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elden\Documents\Repositories\Digital-Currency-Exchange-Routing\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E65B275-0BCB-4A19-894D-D225E81B4432}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D8B7EB-8ADF-475A-A114-066F082351D9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#E#C(无上界)" sheetId="1" r:id="rId1"/>
     <sheet name="子环路消除约束(无上界)" sheetId="2" r:id="rId2"/>
     <sheet name="#E#C(有上界)" sheetId="4" r:id="rId3"/>
+    <sheet name="#E#C(有上界允许1%间隙) " sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="16">
   <si>
     <t xml:space="preserve">        货币种类数量
 交易所数量</t>
@@ -204,7 +205,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -232,10 +233,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2005,6 +2013,1756 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="zh-CN" sz="1050" b="1" i="0" baseline="0">
+                <a:effectLst/>
+                <a:latin typeface="楷体" panose="02010609060101010101" pitchFamily="49" charset="-122"/>
+                <a:ea typeface="楷体" panose="02010609060101010101" pitchFamily="49" charset="-122"/>
+              </a:rPr>
+              <a:t>归一化时间</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1050" b="1" i="0" baseline="0">
+                <a:effectLst/>
+                <a:latin typeface="楷体" panose="02010609060101010101" pitchFamily="49" charset="-122"/>
+                <a:ea typeface="楷体" panose="02010609060101010101" pitchFamily="49" charset="-122"/>
+              </a:rPr>
+              <a:t>(</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="zh-CN" sz="1050" b="1" i="0" baseline="0">
+                <a:effectLst/>
+                <a:latin typeface="楷体" panose="02010609060101010101" pitchFamily="49" charset="-122"/>
+                <a:ea typeface="楷体" panose="02010609060101010101" pitchFamily="49" charset="-122"/>
+              </a:rPr>
+              <a:t>固定货币种类数量</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1050" b="1" i="0" baseline="0">
+                <a:effectLst/>
+                <a:latin typeface="楷体" panose="02010609060101010101" pitchFamily="49" charset="-122"/>
+                <a:ea typeface="楷体" panose="02010609060101010101" pitchFamily="49" charset="-122"/>
+              </a:rPr>
+              <a:t>)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1050">
+              <a:effectLst/>
+              <a:latin typeface="楷体" panose="02010609060101010101" pitchFamily="49" charset="-122"/>
+              <a:ea typeface="楷体" panose="02010609060101010101" pitchFamily="49" charset="-122"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'#E#C(有上界允许1%间隙) '!$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>#E = 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'#E#C(有上界允许1%间隙) '!$I$1:$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>#C = 2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>#C = 3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>#C = 4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>#C = 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'#E#C(有上界允许1%间隙) '!$I$2:$L$2</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>6.9673661727742336E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.22763531687584626</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.43888867907901863</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-772C-4B72-A3B6-B81FA11882C2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'#E#C(有上界允许1%间隙) '!$H$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>#E = 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'#E#C(有上界允许1%间隙) '!$I$1:$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>#C = 2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>#C = 3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>#C = 4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>#C = 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'#E#C(有上界允许1%间隙) '!$I$3:$L$3</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.0203119555457592E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.9375623722383809E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.16337949793255493</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-772C-4B72-A3B6-B81FA11882C2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'#E#C(有上界允许1%间隙) '!$H$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>#E = 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'#E#C(有上界允许1%间隙) '!$I$1:$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>#C = 2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>#C = 3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>#C = 4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>#C = 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'#E#C(有上界允许1%间隙) '!$I$4:$L$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.0619571597334185E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.30302838929216158</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.54648396771501118</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-772C-4B72-A3B6-B81FA11882C2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'#E#C(有上界允许1%间隙) '!$H$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>#E = 4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'#E#C(有上界允许1%间隙) '!$I$1:$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>#C = 2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>#C = 3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>#C = 4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>#C = 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'#E#C(有上界允许1%间隙) '!$I$5:$L$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.0840450746613939E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.4597039200386075E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.24686138690856865</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-772C-4B72-A3B6-B81FA11882C2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'#E#C(有上界允许1%间隙) '!$H$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>#E = 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'#E#C(有上界允许1%间隙) '!$I$1:$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>#C = 2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>#C = 3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>#C = 4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>#C = 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'#E#C(有上界允许1%间隙) '!$I$6:$L$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.3985239793049115E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.6344444263751363E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6072772391618646E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-772C-4B72-A3B6-B81FA11882C2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'#E#C(有上界允许1%间隙) '!$H$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>#E = 6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'#E#C(有上界允许1%间隙) '!$I$1:$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>#C = 2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>#C = 3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>#C = 4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>#C = 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'#E#C(有上界允许1%间隙) '!$I$7:$L$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.0580886581459745E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.8009542083242789E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.8841771528198175E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-772C-4B72-A3B6-B81FA11882C2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'#E#C(有上界允许1%间隙) '!$H$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>#E = 7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'#E#C(有上界允许1%间隙) '!$I$1:$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>#C = 2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>#C = 3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>#C = 4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>#C = 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'#E#C(有上界允许1%间隙) '!$I$8:$L$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>9.502588384990171E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.7817095884786267E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.44736072616048955</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-772C-4B72-A3B6-B81FA11882C2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'#E#C(有上界允许1%间隙) '!$H$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>#E = 8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'#E#C(有上界允许1%间隙) '!$I$1:$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>#C = 2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>#C = 3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>#C = 4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>#C = 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'#E#C(有上界允许1%间隙) '!$I$9:$L$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.1639764473907958E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.3786518149519052E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1258402128701047E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-772C-4B72-A3B6-B81FA11882C2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="663197391"/>
+        <c:axId val="663197807"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="663197391"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="663197807"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="663197807"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="663197391"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1050" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="zh-CN" altLang="en-US" sz="1050" b="1">
+                <a:latin typeface="楷体" panose="02010609060101010101" pitchFamily="49" charset="-122"/>
+                <a:ea typeface="楷体" panose="02010609060101010101" pitchFamily="49" charset="-122"/>
+              </a:rPr>
+              <a:t>归一化时间</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1050" b="1">
+                <a:latin typeface="楷体" panose="02010609060101010101" pitchFamily="49" charset="-122"/>
+                <a:ea typeface="楷体" panose="02010609060101010101" pitchFamily="49" charset="-122"/>
+              </a:rPr>
+              <a:t>(</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="zh-CN" altLang="en-US" sz="1050" b="1">
+                <a:latin typeface="楷体" panose="02010609060101010101" pitchFamily="49" charset="-122"/>
+                <a:ea typeface="楷体" panose="02010609060101010101" pitchFamily="49" charset="-122"/>
+              </a:rPr>
+              <a:t>固定货币种类数量</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1050" b="1">
+                <a:latin typeface="楷体" panose="02010609060101010101" pitchFamily="49" charset="-122"/>
+                <a:ea typeface="楷体" panose="02010609060101010101" pitchFamily="49" charset="-122"/>
+              </a:rPr>
+              <a:t>)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1050" b="1">
+              <a:latin typeface="楷体" panose="02010609060101010101" pitchFamily="49" charset="-122"/>
+              <a:ea typeface="楷体" panose="02010609060101010101" pitchFamily="49" charset="-122"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1050" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'#E#C(有上界允许1%间隙) '!$B$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>#C = 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'#E#C(有上界允许1%间隙) '!$A$13:$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>#E = 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>#E = 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>#E = 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>#E = 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>#E = 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>#E = 6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>#E = 7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>#E = 8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'#E#C(有上界允许1%间隙) '!$B$13:$B$20</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.11674787830207912</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.32369340674021346</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.23416373109456409</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.17637339070882641</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.44020222048783192</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.94120418222343993</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.61768655824385843</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5C52-484B-BA93-1CE8DE1DC606}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'#E#C(有上界允许1%间隙) '!$C$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>#C = 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'#E#C(有上界允许1%间隙) '!$A$13:$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>#E = 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>#E = 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>#E = 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>#E = 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>#E = 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>#E = 6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>#E = 7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>#E = 8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'#E#C(有上界允许1%间隙) '!$C$13:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.11084004527752897</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.13676633444075267</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.35897765954403815</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.60682513801882332</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.7692378418800816</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.51280888224164722</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.67521341326370221</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5C52-484B-BA93-1CE8DE1DC606}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'#E#C(有上界允许1%间隙) '!$D$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>#C = 4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'#E#C(有上界允许1%间隙) '!$A$13:$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>#E = 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>#E = 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>#E = 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>#E = 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>#E = 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>#E = 6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>#E = 7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>#E = 8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'#E#C(有上界允许1%间隙) '!$D$13:$D$20</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.2309318949551147E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.3813935238379592E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1038763550848732</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.34968612954936912</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.4678350900561652E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.77262478173119942</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.74165011862454355</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-5C52-484B-BA93-1CE8DE1DC606}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'#E#C(有上界允许1%间隙) '!$E$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>#C = 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'#E#C(有上界允许1%间隙) '!$A$13:$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>#E = 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>#E = 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>#E = 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>#E = 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>#E = 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>#E = 6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>#E = 7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>#E = 8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'#E#C(有上界允许1%间隙) '!$E$13:$E$20</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.7729742176712668E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6952645429251592E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2016058958874527E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.9546376216492717E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.3304611410406068E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0480065323919732E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.56149516000268318</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-5C52-484B-BA93-1CE8DE1DC606}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="808498559"/>
+        <c:axId val="808498975"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="808498559"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="808498975"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="808498975"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="808498559"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2085,6 +3843,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -2589,6 +4427,1012 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3152,6 +5996,87 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>159543</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>235744</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>188118</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>502444</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{947911D3-3F9D-4113-A5F1-2E62EC164A7B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>621505</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>69056</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>692943</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>145256</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5676A14-8A2C-421E-9E50-BFFEB1B076F2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -3695,14 +6620,14 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="9"/>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11" t="s">
+      <c r="C1" s="12"/>
+      <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11"/>
+      <c r="E1" s="12"/>
     </row>
     <row r="2" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
@@ -3888,7 +6813,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4778A3EF-D417-4E06-BC00-FC009FA5B12B}">
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
@@ -4243,19 +7168,19 @@
       <c r="A10" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="11">
         <f>MAX(B2:B9)</f>
         <v>2.3935079574584898E-2</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="11">
         <f t="shared" ref="C10:E10" si="1">MAX(C2:C9)</f>
         <v>0.51960492134094205</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="11">
         <f t="shared" si="1"/>
         <v>11.026761054992599</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="11">
         <f t="shared" si="1"/>
         <v>4923.1231200000002</v>
       </c>
@@ -4424,4 +7349,579 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90F5ED76-EDB7-43BB-95A8-47FA3BE0CF2D}">
+  <dimension ref="A1:V20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="B2:E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="20.59765625" style="7" customWidth="1"/>
+    <col min="2" max="7" width="10.59765625" style="7"/>
+    <col min="8" max="8" width="20.59765625" style="7" customWidth="1"/>
+    <col min="9" max="16384" width="10.59765625" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6">
+        <v>2</v>
+      </c>
+      <c r="C1" s="6">
+        <v>3</v>
+      </c>
+      <c r="D1" s="6">
+        <v>4</v>
+      </c>
+      <c r="E1" s="6">
+        <v>5</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11">
+        <v>3.9587020874023403E-3</v>
+      </c>
+      <c r="C2" s="11">
+        <v>1.29337310791015E-2</v>
+      </c>
+      <c r="D2" s="11">
+        <v>2.4936676025390601E-2</v>
+      </c>
+      <c r="E2" s="11">
+        <v>5.6817770004272398E-2</v>
+      </c>
+      <c r="F2" s="1">
+        <f>MAX(B2:E2)</f>
+        <v>5.6817770004272398E-2</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="1" cm="1">
+        <f t="array" ref="I2:L2">B2:E2/F2</f>
+        <v>6.9673661727742336E-2</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0.22763531687584626</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0.43888867907901863</v>
+      </c>
+      <c r="L2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="11">
+        <v>1.09758377075195E-2</v>
+      </c>
+      <c r="C3" s="11">
+        <v>1.5959024429321199E-2</v>
+      </c>
+      <c r="D3" s="11">
+        <v>8.87598991394042E-2</v>
+      </c>
+      <c r="E3" s="11">
+        <v>0.54327440261840798</v>
+      </c>
+      <c r="F3" s="1">
+        <f t="shared" ref="F3:F9" si="0">MAX(B3:E3)</f>
+        <v>0.54327440261840798</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="1" cm="1">
+        <f t="array" ref="I3:L3">B3:E3/F3</f>
+        <v>2.0203119555457592E-2</v>
+      </c>
+      <c r="J3" s="1">
+        <v>2.9375623722383809E-2</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0.16337949793255493</v>
+      </c>
+      <c r="L3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" s="11">
+        <v>7.9400539398193307E-3</v>
+      </c>
+      <c r="C4" s="11">
+        <v>0.116688251495361</v>
+      </c>
+      <c r="D4" s="11">
+        <v>0.21043658256530701</v>
+      </c>
+      <c r="E4" s="11">
+        <v>0.385073661804199</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" si="0"/>
+        <v>0.385073661804199</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="1" cm="1">
+        <f t="array" ref="I4:L4">B4:E4/F4</f>
+        <v>2.0619571597334185E-2</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0.30302838929216158</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0.54648396771501118</v>
+      </c>
+      <c r="L4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="11">
+        <v>5.9804916381835903E-3</v>
+      </c>
+      <c r="C5" s="11">
+        <v>4.1888475418090799E-2</v>
+      </c>
+      <c r="D5" s="11">
+        <v>0.70840716361999501</v>
+      </c>
+      <c r="E5" s="11">
+        <v>2.86965560913085</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" si="0"/>
+        <v>2.86965560913085</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="1" cm="1">
+        <f t="array" ref="I5:L5">B5:E5/F5</f>
+        <v>2.0840450746613939E-3</v>
+      </c>
+      <c r="J5" s="1">
+        <v>1.4597039200386075E-2</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0.24686138690856865</v>
+      </c>
+      <c r="L5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="11">
+        <v>1.4926433563232399E-2</v>
+      </c>
+      <c r="C6" s="11">
+        <v>7.0809364318847601E-2</v>
+      </c>
+      <c r="D6" s="11">
+        <v>0.17154455184936501</v>
+      </c>
+      <c r="E6" s="14">
+        <v>10.672990798950099</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="0"/>
+        <v>10.672990798950099</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="1" cm="1">
+        <f t="array" ref="I6:L6">B6:E6/F6</f>
+        <v>1.3985239793049115E-3</v>
+      </c>
+      <c r="J6" s="1">
+        <v>6.6344444263751363E-3</v>
+      </c>
+      <c r="K6" s="1">
+        <v>1.6072772391618646E-2</v>
+      </c>
+      <c r="L6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="6">
+        <v>6</v>
+      </c>
+      <c r="B7" s="11">
+        <v>3.3908128738403299E-2</v>
+      </c>
+      <c r="C7" s="11">
+        <v>8.9761018753051702E-2</v>
+      </c>
+      <c r="D7" s="11">
+        <v>1.5652120113372801</v>
+      </c>
+      <c r="E7" s="15">
+        <v>320.465855836868</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="0"/>
+        <v>320.465855836868</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="1" cm="1">
+        <f t="array" ref="I7:L7">B7:E7/F7</f>
+        <v>1.0580886581459745E-4</v>
+      </c>
+      <c r="J7" s="1">
+        <v>2.8009542083242789E-4</v>
+      </c>
+      <c r="K7" s="1">
+        <v>4.8841771528198175E-3</v>
+      </c>
+      <c r="L7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="6">
+        <v>7</v>
+      </c>
+      <c r="B8" s="11">
+        <v>3.1914472579955999E-2</v>
+      </c>
+      <c r="C8" s="11">
+        <v>5.9838771820068297E-2</v>
+      </c>
+      <c r="D8" s="11">
+        <v>1.50246238708496</v>
+      </c>
+      <c r="E8" s="11">
+        <v>3.3585031032562198</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="0"/>
+        <v>3.3585031032562198</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="1" cm="1">
+        <f t="array" ref="I8:L8">B8:E8/F8</f>
+        <v>9.502588384990171E-3</v>
+      </c>
+      <c r="J8" s="1">
+        <v>1.7817095884786267E-2</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0.44736072616048955</v>
+      </c>
+      <c r="L8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="6">
+        <v>8</v>
+      </c>
+      <c r="B9" s="11">
+        <v>2.0944595336914E-2</v>
+      </c>
+      <c r="C9" s="11">
+        <v>7.8789472579955999E-2</v>
+      </c>
+      <c r="D9" s="11">
+        <v>2.0258371829986501</v>
+      </c>
+      <c r="E9" s="15">
+        <v>179.94002699851899</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="0"/>
+        <v>179.94002699851899</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="1" cm="1">
+        <f t="array" ref="I9:L9">B9:E9/F9</f>
+        <v>1.1639764473907958E-4</v>
+      </c>
+      <c r="J9" s="1">
+        <v>4.3786518149519052E-4</v>
+      </c>
+      <c r="K9" s="1">
+        <v>1.1258402128701047E-2</v>
+      </c>
+      <c r="L9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="11">
+        <f>MAX(B2:B9)</f>
+        <v>3.3908128738403299E-2</v>
+      </c>
+      <c r="C10" s="11">
+        <f t="shared" ref="C10:E10" si="1">MAX(C2:C9)</f>
+        <v>0.116688251495361</v>
+      </c>
+      <c r="D10" s="11">
+        <f t="shared" si="1"/>
+        <v>2.0258371829986501</v>
+      </c>
+      <c r="E10" s="11">
+        <f t="shared" si="1"/>
+        <v>320.465855836868</v>
+      </c>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="12" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="1" cm="1">
+        <f t="array" ref="B13:B20">B2:B9/B10</f>
+        <v>0.11674787830207912</v>
+      </c>
+      <c r="C13" s="1" cm="1">
+        <f t="array" ref="C13:C20">C2:C9/C10</f>
+        <v>0.11084004527752897</v>
+      </c>
+      <c r="D13" s="1" cm="1">
+        <f t="array" ref="D13:D20">D2:D9/D10</f>
+        <v>1.2309318949551147E-2</v>
+      </c>
+      <c r="E13" s="1" cm="1">
+        <f t="array" ref="E13:E20">E2:E9/E10</f>
+        <v>1.7729742176712668E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0.32369340674021346</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.13676633444075267</v>
+      </c>
+      <c r="D14" s="1">
+        <v>4.3813935238379592E-2</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1.6952645429251592E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0.23416373109456409</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0.1038763550848732</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1.2016058958874527E-3</v>
+      </c>
+      <c r="P15" s="13"/>
+    </row>
+    <row r="16" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0.17637339070882641</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.35897765954403815</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0.34968612954936912</v>
+      </c>
+      <c r="E16" s="1">
+        <v>8.9546376216492717E-3</v>
+      </c>
+      <c r="P16" s="13"/>
+    </row>
+    <row r="17" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.44020222048783192</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.60682513801882332</v>
+      </c>
+      <c r="D17" s="1">
+        <v>8.4678350900561652E-2</v>
+      </c>
+      <c r="E17" s="1">
+        <v>3.3304611410406068E-2</v>
+      </c>
+      <c r="O17" s="13"/>
+      <c r="P17" s="13"/>
+      <c r="Q17" s="13"/>
+      <c r="R17" s="13"/>
+      <c r="S17" s="13"/>
+      <c r="T17" s="13"/>
+      <c r="U17" s="13"/>
+      <c r="V17" s="13"/>
+    </row>
+    <row r="18" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0.7692378418800816</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0.77262478173119942</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1</v>
+      </c>
+      <c r="O18" s="13"/>
+      <c r="P18" s="13"/>
+      <c r="Q18" s="13"/>
+      <c r="R18" s="13"/>
+      <c r="S18" s="13"/>
+      <c r="T18" s="13"/>
+      <c r="U18" s="13"/>
+      <c r="V18" s="13"/>
+    </row>
+    <row r="19" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0.94120418222343993</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0.51280888224164722</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0.74165011862454355</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1.0480065323919732E-2</v>
+      </c>
+      <c r="O19" s="13"/>
+      <c r="P19" s="13"/>
+      <c r="Q19" s="13"/>
+      <c r="R19" s="13"/>
+      <c r="S19" s="13"/>
+      <c r="T19" s="13"/>
+      <c r="U19" s="13"/>
+      <c r="V19" s="13"/>
+    </row>
+    <row r="20" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0.61768655824385843</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0.67521341326370221</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0.56149516000268318</v>
+      </c>
+      <c r="O20" s="13"/>
+      <c r="P20" s="13"/>
+      <c r="Q20" s="13"/>
+      <c r="R20" s="13"/>
+      <c r="S20" s="13"/>
+      <c r="T20" s="13"/>
+      <c r="U20" s="13"/>
+      <c r="V20" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added result of running time
</commit_message>
<xml_diff>
--- a/doc/Time.xlsx
+++ b/doc/Time.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elden\Documents\Repositories\Digital-Currency-Exchange-Routing\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE921CA-FF74-44E3-AE2E-E4FACF877625}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74D10C75-E16C-44F8-863C-DA6C4A578EA4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="345" windowWidth="28695" windowHeight="15255" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1290" yWindow="848" windowWidth="28695" windowHeight="15255" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#E#C(无上界)" sheetId="1" r:id="rId1"/>
     <sheet name="子环路消除约束(无上界)" sheetId="2" r:id="rId2"/>
     <sheet name="#E#C(有上界允许1%间隙) " sheetId="5" r:id="rId3"/>
     <sheet name="间隙研究" sheetId="11" r:id="rId4"/>
-    <sheet name="#E#C(有上界允许4%间隙)  " sheetId="13" r:id="rId5"/>
+    <sheet name="#E#C(有上界允许5%间隙)  " sheetId="13" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -305,9 +305,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -337,6 +334,9 @@
     </xf>
     <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4870,14 +4870,14 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="9"/>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23" t="s">
+      <c r="C1" s="33"/>
+      <c r="D1" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="23"/>
+      <c r="E1" s="33"/>
     </row>
     <row r="2" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
@@ -5793,7 +5793,7 @@
   <dimension ref="A1:X18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="J11" sqref="A1:J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -5843,36 +5843,36 @@
       <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="26">
+      <c r="B2" s="25">
         <v>6.9842338562011701E-3</v>
       </c>
-      <c r="C2" s="26">
+      <c r="C2" s="25">
         <v>2.490234375E-2</v>
       </c>
-      <c r="D2" s="26">
+      <c r="D2" s="25">
         <v>2.1939992904662999E-2</v>
       </c>
-      <c r="E2" s="26">
+      <c r="E2" s="25">
         <v>1.9947767257690398E-2</v>
       </c>
-      <c r="F2" s="26">
+      <c r="F2" s="25">
         <v>3.2912492752075098E-2</v>
       </c>
-      <c r="G2" s="26">
+      <c r="G2" s="25">
         <v>0.14708733558654699</v>
       </c>
-      <c r="H2" s="27">
+      <c r="H2" s="26">
         <v>6.3797712326049805E-2</v>
       </c>
-      <c r="I2" s="33">
+      <c r="I2" s="32">
         <v>0.1845064163208</v>
       </c>
-      <c r="J2" s="24">
+      <c r="J2" s="23">
         <v>0.35505056381225503</v>
       </c>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="25"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="24"/>
       <c r="N2" s="22"/>
       <c r="O2" s="22"/>
       <c r="P2" s="22"/>
@@ -5889,32 +5889,32 @@
       <c r="A3" s="6">
         <v>2</v>
       </c>
-      <c r="B3" s="26">
+      <c r="B3" s="25">
         <v>7.9748630523681606E-3</v>
       </c>
-      <c r="C3" s="26">
+      <c r="C3" s="25">
         <v>1.49612426757812E-2</v>
       </c>
-      <c r="D3" s="26">
+      <c r="D3" s="25">
         <v>5.6848764419555602E-2</v>
       </c>
-      <c r="E3" s="26">
+      <c r="E3" s="25">
         <v>0.110703945159912</v>
       </c>
-      <c r="F3" s="26">
+      <c r="F3" s="25">
         <v>1.8789758682250901</v>
       </c>
-      <c r="G3" s="26">
+      <c r="G3" s="25">
         <v>19.918958425521801</v>
       </c>
-      <c r="H3" s="27">
+      <c r="H3" s="26">
         <v>460.84453129768298</v>
       </c>
-      <c r="I3" s="28"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="25"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="24"/>
       <c r="N3" s="22"/>
       <c r="O3" s="22"/>
       <c r="P3" s="22"/>
@@ -5931,30 +5931,30 @@
       <c r="A4" s="6">
         <v>3</v>
       </c>
-      <c r="B4" s="26">
+      <c r="B4" s="25">
         <v>7.9474449157714792E-3</v>
       </c>
-      <c r="C4" s="26">
+      <c r="C4" s="25">
         <v>2.7930736541747998E-2</v>
       </c>
-      <c r="D4" s="26">
+      <c r="D4" s="25">
         <v>9.17205810546875E-2</v>
       </c>
-      <c r="E4" s="26">
+      <c r="E4" s="25">
         <v>0.33307075500488198</v>
       </c>
-      <c r="F4" s="26">
+      <c r="F4" s="25">
         <v>45.396625995635901</v>
       </c>
-      <c r="G4" s="26">
+      <c r="G4" s="25">
         <v>54.328840494155799</v>
       </c>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="32"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
-      <c r="M4" s="25"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="24"/>
       <c r="N4" s="22"/>
       <c r="O4" s="22"/>
       <c r="P4" s="22"/>
@@ -5971,28 +5971,28 @@
       <c r="A5" s="6">
         <v>4</v>
       </c>
-      <c r="B5" s="26">
+      <c r="B5" s="25">
         <v>9.9389553070068307E-3</v>
       </c>
-      <c r="C5" s="26">
+      <c r="C5" s="25">
         <v>1.5933036804199201E-2</v>
       </c>
-      <c r="D5" s="26">
+      <c r="D5" s="25">
         <v>0.17351102828979401</v>
       </c>
-      <c r="E5" s="26">
+      <c r="E5" s="25">
         <v>4.1738381385803196</v>
       </c>
-      <c r="F5" s="26">
+      <c r="F5" s="25">
         <v>8.7475855350494296</v>
       </c>
-      <c r="G5" s="29"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="24"/>
-      <c r="L5" s="24"/>
-      <c r="M5" s="25"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="24"/>
       <c r="N5" s="22"/>
       <c r="O5" s="22"/>
       <c r="P5" s="22"/>
@@ -6009,28 +6009,28 @@
       <c r="A6" s="6">
         <v>5</v>
       </c>
-      <c r="B6" s="26">
+      <c r="B6" s="25">
         <v>5.9838294982910104E-3</v>
       </c>
-      <c r="C6" s="26">
+      <c r="C6" s="25">
         <v>3.1914710998535101E-2</v>
       </c>
-      <c r="D6" s="26">
+      <c r="D6" s="25">
         <v>0.22041082382202101</v>
       </c>
-      <c r="E6" s="26">
+      <c r="E6" s="25">
         <v>1.31448554992675</v>
       </c>
-      <c r="F6" s="26">
+      <c r="F6" s="25">
         <v>15.600257873535099</v>
       </c>
-      <c r="G6" s="29"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
-      <c r="M6" s="25"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="24"/>
       <c r="N6" s="22"/>
       <c r="O6" s="12"/>
       <c r="P6" s="12"/>
@@ -6047,30 +6047,30 @@
       <c r="A7" s="6">
         <v>6</v>
       </c>
-      <c r="B7" s="26">
+      <c r="B7" s="25">
         <v>1.29261016845703E-2</v>
       </c>
-      <c r="C7" s="26">
+      <c r="C7" s="25">
         <v>4.0888071060180602E-2</v>
       </c>
-      <c r="D7" s="26">
+      <c r="D7" s="25">
         <v>5.3852319717407199E-2</v>
       </c>
-      <c r="E7" s="26">
+      <c r="E7" s="25">
         <v>0.19946527481079099</v>
       </c>
-      <c r="F7" s="27">
+      <c r="F7" s="26">
         <v>1.7732625007629299</v>
       </c>
-      <c r="G7" s="26">
+      <c r="G7" s="25">
         <v>4189.2489449882496</v>
       </c>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="32"/>
-      <c r="K7" s="24"/>
-      <c r="L7" s="24"/>
-      <c r="M7" s="25"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="24"/>
       <c r="N7" s="22"/>
       <c r="O7" s="12"/>
       <c r="P7" s="12"/>
@@ -6087,28 +6087,28 @@
       <c r="A8" s="6">
         <v>7</v>
       </c>
-      <c r="B8" s="30">
+      <c r="B8" s="29">
         <v>1.5924215316772398E-2</v>
       </c>
-      <c r="C8" s="26">
+      <c r="C8" s="25">
         <v>7.9783678054809501E-2</v>
       </c>
-      <c r="D8" s="30">
+      <c r="D8" s="29">
         <v>0.61734938621520896</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E8" s="26">
         <v>446.27465629577603</v>
       </c>
-      <c r="F8" s="27">
+      <c r="F8" s="26">
         <v>9490.6387329101508</v>
       </c>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="32"/>
-      <c r="K8" s="24"/>
-      <c r="L8" s="24"/>
-      <c r="M8" s="25"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="24"/>
       <c r="N8" s="22"/>
       <c r="O8" s="12"/>
       <c r="P8" s="12"/>
@@ -6125,26 +6125,26 @@
       <c r="A9" s="6">
         <v>8</v>
       </c>
-      <c r="B9" s="27">
+      <c r="B9" s="26">
         <v>1.19342803955078E-2</v>
       </c>
-      <c r="C9" s="27">
+      <c r="C9" s="26">
         <v>4.7877311706542899E-2</v>
       </c>
-      <c r="D9" s="27">
+      <c r="D9" s="26">
         <v>0.94643282890319802</v>
       </c>
-      <c r="E9" s="27">
+      <c r="E9" s="26">
         <v>213.494951963424</v>
       </c>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="31"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="25"/>
-      <c r="L9" s="25"/>
-      <c r="M9" s="25"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="24"/>
       <c r="N9" s="22"/>
       <c r="O9" s="12"/>
       <c r="P9" s="12"/>
@@ -6161,26 +6161,26 @@
       <c r="A10" s="6">
         <v>9</v>
       </c>
-      <c r="B10" s="27">
+      <c r="B10" s="26">
         <v>1.4962434768676701E-2</v>
       </c>
-      <c r="C10" s="27">
+      <c r="C10" s="26">
         <v>4.2883872985839802E-2</v>
       </c>
-      <c r="D10" s="27">
+      <c r="D10" s="26">
         <v>0.94447374343872004</v>
       </c>
-      <c r="E10" s="27">
+      <c r="E10" s="26">
         <v>41.717653989791799</v>
       </c>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="31"/>
-      <c r="J10" s="31"/>
-      <c r="K10" s="25"/>
-      <c r="L10" s="25"/>
-      <c r="M10" s="25"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
       <c r="N10" s="22"/>
       <c r="O10" s="12"/>
       <c r="P10" s="12"/>
@@ -6197,24 +6197,24 @@
       <c r="A11" s="6">
         <v>10</v>
       </c>
-      <c r="B11" s="27">
+      <c r="B11" s="26">
         <v>8.9762210845947196E-3</v>
       </c>
-      <c r="C11" s="27">
+      <c r="C11" s="26">
         <v>0.14458012580871499</v>
       </c>
-      <c r="D11" s="27">
+      <c r="D11" s="26">
         <v>1.2376568317413299</v>
       </c>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="25"/>
-      <c r="L11" s="25"/>
-      <c r="M11" s="25"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
       <c r="N11" s="22"/>
       <c r="O11" s="12"/>
       <c r="P11" s="12"/>
@@ -6229,33 +6229,33 @@
     </row>
     <row r="12" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="6"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="25"/>
-      <c r="M12" s="25"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="24"/>
     </row>
     <row r="13" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="6"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="25"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="25"/>
-      <c r="L13" s="25"/>
-      <c r="M13" s="25"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="24"/>
+      <c r="M13" s="24"/>
       <c r="N13" s="22"/>
       <c r="O13" s="22"/>
       <c r="P13" s="22"/>
@@ -6269,18 +6269,18 @@
     </row>
     <row r="14" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="6"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="25"/>
-      <c r="L14" s="25"/>
-      <c r="M14" s="25"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24"/>
+      <c r="L14" s="24"/>
+      <c r="M14" s="24"/>
       <c r="N14" s="22"/>
       <c r="O14" s="22"/>
       <c r="P14" s="22"/>
@@ -6294,18 +6294,18 @@
     </row>
     <row r="15" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="6"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="27"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="25"/>
-      <c r="L15" s="25"/>
-      <c r="M15" s="25"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
+      <c r="L15" s="24"/>
+      <c r="M15" s="24"/>
       <c r="P15" s="12"/>
       <c r="Q15" s="12"/>
       <c r="R15" s="12"/>

</xml_diff>